<commit_message>
Converted LSR mapping CSV to Excel
</commit_message>
<xml_diff>
--- a/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
+++ b/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
@@ -17,17 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,57 +422,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Extraction sheet name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Data file (doi)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>LSR no.</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Extraction sheet dimension</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Variable to extract</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Understandable label for database</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Class ID</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Class  label</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Class definition</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Parent class</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Ontology spreadsheet</t>
         </is>

</xml_diff>